<commit_message>
add half checklist from surname field
</commit_message>
<xml_diff>
--- a/Form_Checklist.xlsx
+++ b/Form_Checklist.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="172">
   <si>
     <t xml:space="preserve">Ubuntu 20.04.4 Focal, Google Chrome </t>
   </si>
@@ -51,7 +51,7 @@
     <t xml:space="preserve">Bug ID</t>
   </si>
   <si>
-    <t xml:space="preserve">Поле Name</t>
+    <t xml:space="preserve">1. Поле Name</t>
   </si>
   <si>
     <t xml:space="preserve">Ввести 1 латинский символ</t>
@@ -424,6 +424,120 @@
   </si>
   <si>
     <t xml:space="preserve">ID_1.17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Поле Surname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Akh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Akhl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ввести 11 латинских символa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Akhlamionok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127 symb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ввести Surname на кириллице</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ахламёнок</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Написать Surname в верхнем регистре</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AKHLAMIONOK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Написать Surname в нижнем регистре</t>
+  </si>
+  <si>
+    <t xml:space="preserve">akhlamionok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Написать Surname с использованием разрешенных спецсимволов</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A-k_hla-mionok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Написать Surname с использованием запрещенных спецсимволов</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@khl@mionok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Написать Surname латиницей с цифрами</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Akhla123mionok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Написать  Surname кириллицей с цифрами</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ахла123мёнок</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Написать латинский Surname с цифрами в начале</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123Akhlamionok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Написать латинский Surname с цифрами в конце</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Akhlamionok123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123Ахламёнок</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ахламёнок123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Написать Surname латиницей с разрешенными спецсимволами в начале</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-Akhlamionok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Написать Surname латиницей с разрешенными спецсимволами в конце</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Akhlamionok_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Написать Sruname латиницей с разрешенными спецсимволами подряд в начале</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Написать Surname латиницей с разрешенными спецсимволами подряд в середине</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Написать Surname латиницей с разрешенными спецсимволами подряд в конце</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Скопировать валидное значение Surname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ввести в поле только разрешенные спецсимволы</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“Surname”</t>
   </si>
 </sst>
 </file>
@@ -433,7 +547,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -494,6 +608,12 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="4">
@@ -557,7 +677,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -567,7 +687,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -614,12 +734,12 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -632,6 +752,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -711,20 +835,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AA43"/>
+  <dimension ref="A1:AA82"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I32" activeCellId="0" sqref="I32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D67" activeCellId="0" sqref="D67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="39.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.5"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="12.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="16.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="21.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="49.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="49.61"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="7" style="4" width="12.63"/>
   </cols>
   <sheetData>
@@ -840,7 +964,7 @@
       </c>
       <c r="H4" s="11"/>
     </row>
-    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="n">
         <v>2</v>
       </c>
@@ -848,7 +972,7 @@
         <v>16</v>
       </c>
       <c r="C5" s="6"/>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="11" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="12" t="s">
@@ -857,14 +981,14 @@
       <c r="F5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="14" t="s">
         <v>19</v>
       </c>
       <c r="H5" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="n">
         <v>3</v>
       </c>
@@ -872,7 +996,7 @@
         <v>21</v>
       </c>
       <c r="C6" s="6"/>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="11" t="s">
         <v>22</v>
       </c>
       <c r="E6" s="12" t="s">
@@ -881,14 +1005,14 @@
       <c r="F6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="14" t="s">
         <v>19</v>
       </c>
       <c r="H6" s="11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="n">
         <v>4</v>
       </c>
@@ -896,13 +1020,13 @@
         <v>24</v>
       </c>
       <c r="C7" s="6"/>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="11" t="s">
         <v>25</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="15" t="s">
         <v>26</v>
       </c>
       <c r="G7" s="13" t="s">
@@ -910,7 +1034,7 @@
       </c>
       <c r="H7" s="11"/>
     </row>
-    <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="11" t="n">
         <v>5</v>
       </c>
@@ -918,13 +1042,13 @@
         <v>27</v>
       </c>
       <c r="C8" s="6"/>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="11" t="s">
         <v>28</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="15" t="s">
         <v>29</v>
       </c>
       <c r="G8" s="13" t="s">
@@ -932,7 +1056,7 @@
       </c>
       <c r="H8" s="11"/>
     </row>
-    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="n">
         <v>6</v>
       </c>
@@ -940,21 +1064,21 @@
         <v>30</v>
       </c>
       <c r="C9" s="6"/>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="11" t="s">
         <v>31</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G9" s="14" t="s">
         <v>19</v>
       </c>
       <c r="H9" s="11"/>
     </row>
-    <row r="10" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="11" t="n">
         <v>7</v>
       </c>
@@ -962,21 +1086,21 @@
         <v>33</v>
       </c>
       <c r="C10" s="6"/>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="11" t="s">
         <v>34</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="14" t="s">
         <v>19</v>
       </c>
       <c r="H10" s="11"/>
     </row>
-    <row r="11" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="11" t="n">
         <v>8</v>
       </c>
@@ -984,13 +1108,13 @@
         <v>35</v>
       </c>
       <c r="C11" s="6"/>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="11" t="s">
         <v>36</v>
       </c>
       <c r="E11" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="15" t="s">
         <v>32</v>
       </c>
       <c r="G11" s="13" t="s">
@@ -1006,13 +1130,13 @@
         <v>37</v>
       </c>
       <c r="C12" s="6"/>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="11" t="s">
         <v>38</v>
       </c>
       <c r="E12" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="15" t="s">
         <v>32</v>
       </c>
       <c r="G12" s="13" t="s">
@@ -1020,7 +1144,7 @@
       </c>
       <c r="H12" s="16"/>
     </row>
-    <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="n">
         <v>10</v>
       </c>
@@ -1028,16 +1152,16 @@
         <v>39</v>
       </c>
       <c r="C13" s="6"/>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="11" t="s">
         <v>40</v>
       </c>
       <c r="E13" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="G13" s="15" t="s">
+      <c r="G13" s="14" t="s">
         <v>19</v>
       </c>
       <c r="H13" s="11"/>
@@ -1050,13 +1174,13 @@
         <v>42</v>
       </c>
       <c r="C14" s="6"/>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="11" t="s">
         <v>43</v>
       </c>
       <c r="E14" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="15" t="s">
         <v>44</v>
       </c>
       <c r="G14" s="13" t="s">
@@ -1072,13 +1196,13 @@
         <v>45</v>
       </c>
       <c r="C15" s="6"/>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="11" t="s">
         <v>46</v>
       </c>
       <c r="E15" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="F15" s="15" t="s">
         <v>47</v>
       </c>
       <c r="G15" s="13" t="s">
@@ -1125,7 +1249,7 @@
       <c r="F17" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="G17" s="15" t="s">
+      <c r="G17" s="14" t="s">
         <v>19</v>
       </c>
       <c r="H17" s="16" t="s">
@@ -1140,7 +1264,7 @@
         <v>55</v>
       </c>
       <c r="C18" s="6"/>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E18" s="12" t="s">
@@ -1162,7 +1286,7 @@
         <v>58</v>
       </c>
       <c r="C19" s="6"/>
-      <c r="D19" s="14" t="s">
+      <c r="D19" s="11" t="s">
         <v>59</v>
       </c>
       <c r="E19" s="12" t="s">
@@ -1171,7 +1295,7 @@
       <c r="F19" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="G19" s="15" t="s">
+      <c r="G19" s="14" t="s">
         <v>19</v>
       </c>
       <c r="H19" s="16" t="s">
@@ -1230,7 +1354,7 @@
         <v>68</v>
       </c>
       <c r="C22" s="6"/>
-      <c r="D22" s="14" t="s">
+      <c r="D22" s="11" t="s">
         <v>69</v>
       </c>
       <c r="E22" s="12" t="s">
@@ -1239,7 +1363,7 @@
       <c r="F22" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="G22" s="15" t="s">
+      <c r="G22" s="14" t="s">
         <v>19</v>
       </c>
       <c r="H22" s="16" t="s">
@@ -1254,7 +1378,7 @@
         <v>72</v>
       </c>
       <c r="C23" s="6"/>
-      <c r="D23" s="14" t="s">
+      <c r="D23" s="11" t="s">
         <v>73</v>
       </c>
       <c r="E23" s="12" t="s">
@@ -1263,7 +1387,7 @@
       <c r="F23" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="G23" s="15" t="s">
+      <c r="G23" s="14" t="s">
         <v>19</v>
       </c>
       <c r="H23" s="16" t="s">
@@ -1287,7 +1411,7 @@
       <c r="F24" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="G24" s="15" t="s">
+      <c r="G24" s="14" t="s">
         <v>19</v>
       </c>
       <c r="H24" s="16" t="s">
@@ -1311,7 +1435,7 @@
       <c r="F25" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="G25" s="15" t="s">
+      <c r="G25" s="14" t="s">
         <v>19</v>
       </c>
       <c r="H25" s="16" t="s">
@@ -1335,7 +1459,7 @@
       <c r="F26" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="G26" s="15" t="s">
+      <c r="G26" s="14" t="s">
         <v>19</v>
       </c>
       <c r="H26" s="16" t="s">
@@ -1359,7 +1483,7 @@
       <c r="F27" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="G27" s="15" t="s">
+      <c r="G27" s="14" t="s">
         <v>19</v>
       </c>
       <c r="H27" s="16" t="s">
@@ -1383,7 +1507,7 @@
       <c r="F28" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="G28" s="15" t="s">
+      <c r="G28" s="14" t="s">
         <v>19</v>
       </c>
       <c r="H28" s="16" t="s">
@@ -1398,13 +1522,13 @@
         <v>96</v>
       </c>
       <c r="C29" s="6"/>
-      <c r="D29" s="14" t="s">
+      <c r="D29" s="11" t="s">
         <v>97</v>
       </c>
       <c r="E29" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F29" s="14" t="s">
+      <c r="F29" s="15" t="s">
         <v>47</v>
       </c>
       <c r="G29" s="13" t="s">
@@ -1420,7 +1544,7 @@
         <v>98</v>
       </c>
       <c r="C30" s="6"/>
-      <c r="D30" s="14"/>
+      <c r="D30" s="11"/>
       <c r="E30" s="12" t="s">
         <v>99</v>
       </c>
@@ -1438,7 +1562,7 @@
         <v>100</v>
       </c>
       <c r="C31" s="6"/>
-      <c r="D31" s="14"/>
+      <c r="D31" s="11"/>
       <c r="E31" s="12" t="s">
         <v>101</v>
       </c>
@@ -1456,7 +1580,7 @@
         <v>102</v>
       </c>
       <c r="C32" s="6"/>
-      <c r="D32" s="14"/>
+      <c r="D32" s="11"/>
       <c r="E32" s="12" t="s">
         <v>103</v>
       </c>
@@ -1474,7 +1598,7 @@
         <v>104</v>
       </c>
       <c r="C33" s="6"/>
-      <c r="D33" s="14"/>
+      <c r="D33" s="11"/>
       <c r="E33" s="12" t="s">
         <v>105</v>
       </c>
@@ -1492,7 +1616,7 @@
         <v>106</v>
       </c>
       <c r="C34" s="6"/>
-      <c r="D34" s="14"/>
+      <c r="D34" s="11"/>
       <c r="E34" s="12" t="s">
         <v>107</v>
       </c>
@@ -1510,14 +1634,14 @@
         <v>108</v>
       </c>
       <c r="C35" s="6"/>
-      <c r="D35" s="14"/>
+      <c r="D35" s="11"/>
       <c r="E35" s="12" t="s">
         <v>109</v>
       </c>
       <c r="F35" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="G35" s="15" t="s">
+      <c r="G35" s="14" t="s">
         <v>19</v>
       </c>
       <c r="H35" s="16" t="s">
@@ -1532,14 +1656,14 @@
         <v>112</v>
       </c>
       <c r="C36" s="6"/>
-      <c r="D36" s="14"/>
+      <c r="D36" s="11"/>
       <c r="E36" s="12" t="s">
         <v>113</v>
       </c>
       <c r="F36" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="G36" s="15" t="s">
+      <c r="G36" s="14" t="s">
         <v>19</v>
       </c>
       <c r="H36" s="16" t="s">
@@ -1554,13 +1678,13 @@
         <v>115</v>
       </c>
       <c r="C37" s="6"/>
-      <c r="D37" s="14" t="n">
+      <c r="D37" s="11" t="n">
         <v>123456789</v>
       </c>
       <c r="E37" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="F37" s="14" t="s">
+      <c r="F37" s="15" t="s">
         <v>117</v>
       </c>
       <c r="G37" s="13" t="s">
@@ -1585,7 +1709,7 @@
       <c r="F38" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="G38" s="15" t="s">
+      <c r="G38" s="14" t="s">
         <v>19</v>
       </c>
       <c r="H38" s="16" t="s">
@@ -1600,7 +1724,7 @@
         <v>122</v>
       </c>
       <c r="C39" s="6"/>
-      <c r="D39" s="14" t="s">
+      <c r="D39" s="11" t="s">
         <v>123</v>
       </c>
       <c r="E39" s="12" t="s">
@@ -1609,7 +1733,7 @@
       <c r="F39" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="G39" s="15" t="s">
+      <c r="G39" s="14" t="s">
         <v>19</v>
       </c>
       <c r="H39" s="16" t="s">
@@ -1624,7 +1748,7 @@
         <v>126</v>
       </c>
       <c r="C40" s="6"/>
-      <c r="D40" s="14" t="s">
+      <c r="D40" s="11" t="s">
         <v>127</v>
       </c>
       <c r="E40" s="12" t="s">
@@ -1633,7 +1757,7 @@
       <c r="F40" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="G40" s="15" t="s">
+      <c r="G40" s="14" t="s">
         <v>19</v>
       </c>
       <c r="H40" s="16" t="s">
@@ -1648,14 +1772,14 @@
         <v>130</v>
       </c>
       <c r="C41" s="18"/>
-      <c r="D41" s="14"/>
+      <c r="D41" s="11"/>
       <c r="E41" s="12" t="s">
         <v>131</v>
       </c>
       <c r="F41" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="G41" s="15" t="s">
+      <c r="G41" s="14" t="s">
         <v>19</v>
       </c>
       <c r="H41" s="16" t="s">
@@ -1668,7 +1792,7 @@
       </c>
       <c r="B42" s="12"/>
       <c r="C42" s="18"/>
-      <c r="D42" s="14"/>
+      <c r="D42" s="11"/>
       <c r="E42" s="12"/>
       <c r="F42" s="17"/>
       <c r="G42" s="16"/>
@@ -1680,16 +1804,688 @@
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="18"/>
-      <c r="D43" s="14"/>
+      <c r="D43" s="11"/>
       <c r="E43" s="12"/>
       <c r="F43" s="17"/>
       <c r="G43" s="16"/>
       <c r="H43" s="16"/>
     </row>
+    <row r="44" customFormat="false" ht="42.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="B44" s="10"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
+      <c r="H44" s="10"/>
+    </row>
+    <row r="45" customFormat="false" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D45" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="E45" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F45" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G45" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H45" s="11"/>
+    </row>
+    <row r="46" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C46" s="6"/>
+      <c r="D46" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="E46" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F46" s="17"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="16"/>
+    </row>
+    <row r="47" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C47" s="6"/>
+      <c r="D47" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="E47" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F47" s="17"/>
+      <c r="G47" s="16"/>
+      <c r="H47" s="16"/>
+    </row>
+    <row r="48" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C48" s="6"/>
+      <c r="D48" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F48" s="17"/>
+      <c r="G48" s="16"/>
+      <c r="H48" s="16"/>
+    </row>
+    <row r="49" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="C49" s="6"/>
+      <c r="D49" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="E49" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F49" s="17"/>
+      <c r="G49" s="16"/>
+      <c r="H49" s="16"/>
+    </row>
+    <row r="50" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C50" s="6"/>
+      <c r="D50" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F50" s="17"/>
+      <c r="G50" s="16"/>
+      <c r="H50" s="16"/>
+    </row>
+    <row r="51" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="11" t="n">
+        <v>7</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C51" s="6"/>
+      <c r="D51" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E51" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F51" s="17"/>
+      <c r="G51" s="16"/>
+      <c r="H51" s="16"/>
+    </row>
+    <row r="52" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="11" t="n">
+        <v>8</v>
+      </c>
+      <c r="B52" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C52" s="6"/>
+      <c r="D52" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E52" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F52" s="17"/>
+      <c r="G52" s="16"/>
+      <c r="H52" s="16"/>
+    </row>
+    <row r="53" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="11" t="n">
+        <v>9</v>
+      </c>
+      <c r="B53" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C53" s="6"/>
+      <c r="D53" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E53" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F53" s="17"/>
+      <c r="G53" s="16"/>
+      <c r="H53" s="16"/>
+    </row>
+    <row r="54" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B54" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="C54" s="6"/>
+      <c r="D54" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="E54" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F54" s="17"/>
+      <c r="G54" s="16"/>
+      <c r="H54" s="16"/>
+    </row>
+    <row r="55" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="11" t="n">
+        <v>11</v>
+      </c>
+      <c r="B55" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="C55" s="6"/>
+      <c r="D55" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E55" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F55" s="17"/>
+      <c r="G55" s="16"/>
+      <c r="H55" s="16"/>
+    </row>
+    <row r="56" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="11" t="n">
+        <v>12</v>
+      </c>
+      <c r="B56" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="C56" s="6"/>
+      <c r="D56" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="E56" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F56" s="17"/>
+      <c r="G56" s="16"/>
+      <c r="H56" s="16"/>
+    </row>
+    <row r="57" customFormat="false" ht="27.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="11" t="n">
+        <v>13</v>
+      </c>
+      <c r="B57" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="C57" s="6"/>
+      <c r="D57" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="E57" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F57" s="17"/>
+      <c r="G57" s="16"/>
+      <c r="H57" s="16"/>
+    </row>
+    <row r="58" customFormat="false" ht="27.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="11" t="n">
+        <v>14</v>
+      </c>
+      <c r="B58" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="C58" s="6"/>
+      <c r="D58" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="E58" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F58" s="17"/>
+      <c r="G58" s="16"/>
+      <c r="H58" s="16"/>
+    </row>
+    <row r="59" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="11" t="n">
+        <v>15</v>
+      </c>
+      <c r="B59" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="C59" s="6"/>
+      <c r="D59" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="E59" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F59" s="17"/>
+      <c r="G59" s="16"/>
+      <c r="H59" s="16"/>
+    </row>
+    <row r="60" customFormat="false" ht="27.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="11" t="n">
+        <v>16</v>
+      </c>
+      <c r="B60" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="C60" s="6"/>
+      <c r="D60" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="E60" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F60" s="17"/>
+      <c r="G60" s="16"/>
+      <c r="H60" s="16"/>
+    </row>
+    <row r="61" customFormat="false" ht="27.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="11" t="n">
+        <v>17</v>
+      </c>
+      <c r="B61" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="C61" s="6"/>
+      <c r="D61" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="E61" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F61" s="17"/>
+      <c r="G61" s="16"/>
+      <c r="H61" s="16"/>
+    </row>
+    <row r="62" customFormat="false" ht="27.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="11" t="n">
+        <v>18</v>
+      </c>
+      <c r="B62" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="C62" s="6"/>
+      <c r="D62" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="E62" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F62" s="17"/>
+      <c r="G62" s="16"/>
+      <c r="H62" s="16"/>
+    </row>
+    <row r="63" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="11" t="n">
+        <v>19</v>
+      </c>
+      <c r="B63" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C63" s="6"/>
+      <c r="D63" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="E63" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F63" s="17"/>
+      <c r="G63" s="16"/>
+      <c r="H63" s="16"/>
+    </row>
+    <row r="64" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="B64" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C64" s="6"/>
+      <c r="D64" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="E64" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F64" s="17"/>
+      <c r="G64" s="16"/>
+      <c r="H64" s="16"/>
+    </row>
+    <row r="65" customFormat="false" ht="39.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="11" t="n">
+        <v>21</v>
+      </c>
+      <c r="B65" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="C65" s="6"/>
+      <c r="D65" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="E65" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F65" s="17"/>
+      <c r="G65" s="16"/>
+      <c r="H65" s="16"/>
+    </row>
+    <row r="66" customFormat="false" ht="27.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="11" t="n">
+        <v>22</v>
+      </c>
+      <c r="B66" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="C66" s="6"/>
+      <c r="D66" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="E66" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F66" s="17"/>
+      <c r="G66" s="16"/>
+      <c r="H66" s="16"/>
+    </row>
+    <row r="67" customFormat="false" ht="39.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="11" t="n">
+        <v>23</v>
+      </c>
+      <c r="B67" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="C67" s="6"/>
+      <c r="D67" s="11"/>
+      <c r="E67" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F67" s="17"/>
+      <c r="G67" s="16"/>
+      <c r="H67" s="16"/>
+    </row>
+    <row r="68" customFormat="false" ht="39.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="11" t="n">
+        <v>24</v>
+      </c>
+      <c r="B68" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="C68" s="6"/>
+      <c r="D68" s="11"/>
+      <c r="E68" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F68" s="17"/>
+      <c r="G68" s="16"/>
+      <c r="H68" s="16"/>
+    </row>
+    <row r="69" customFormat="false" ht="39.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="11" t="n">
+        <v>25</v>
+      </c>
+      <c r="B69" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="C69" s="6"/>
+      <c r="D69" s="11"/>
+      <c r="E69" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F69" s="17"/>
+      <c r="G69" s="16"/>
+      <c r="H69" s="16"/>
+    </row>
+    <row r="70" customFormat="false" ht="27.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="11" t="n">
+        <v>26</v>
+      </c>
+      <c r="B70" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="C70" s="6"/>
+      <c r="D70" s="11"/>
+      <c r="E70" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F70" s="17"/>
+      <c r="G70" s="16"/>
+      <c r="H70" s="16"/>
+    </row>
+    <row r="71" customFormat="false" ht="27.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="11" t="n">
+        <v>27</v>
+      </c>
+      <c r="B71" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="C71" s="6"/>
+      <c r="D71" s="11"/>
+      <c r="E71" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="F71" s="17"/>
+      <c r="G71" s="16"/>
+      <c r="H71" s="16"/>
+    </row>
+    <row r="72" customFormat="false" ht="27.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="11" t="n">
+        <v>28</v>
+      </c>
+      <c r="B72" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="C72" s="6"/>
+      <c r="D72" s="11"/>
+      <c r="E72" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="F72" s="17"/>
+      <c r="G72" s="16"/>
+      <c r="H72" s="16"/>
+    </row>
+    <row r="73" customFormat="false" ht="27.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="11" t="n">
+        <v>29</v>
+      </c>
+      <c r="B73" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="C73" s="6"/>
+      <c r="D73" s="11"/>
+      <c r="E73" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="F73" s="17"/>
+      <c r="G73" s="16"/>
+      <c r="H73" s="16"/>
+    </row>
+    <row r="74" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="11" t="n">
+        <v>30</v>
+      </c>
+      <c r="B74" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="C74" s="6"/>
+      <c r="D74" s="11"/>
+      <c r="E74" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="F74" s="17"/>
+      <c r="G74" s="16"/>
+      <c r="H74" s="16"/>
+    </row>
+    <row r="75" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="11" t="n">
+        <v>31</v>
+      </c>
+      <c r="B75" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="C75" s="6"/>
+      <c r="D75" s="11"/>
+      <c r="E75" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="F75" s="17"/>
+      <c r="G75" s="16"/>
+      <c r="H75" s="16"/>
+    </row>
+    <row r="76" customFormat="false" ht="27.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="11" t="n">
+        <v>32</v>
+      </c>
+      <c r="B76" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="C76" s="6"/>
+      <c r="D76" s="11"/>
+      <c r="E76" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="F76" s="17"/>
+      <c r="G76" s="16"/>
+      <c r="H76" s="16"/>
+    </row>
+    <row r="77" customFormat="false" ht="27.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="11" t="n">
+        <v>33</v>
+      </c>
+      <c r="B77" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="C77" s="6"/>
+      <c r="D77" s="11"/>
+      <c r="E77" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="F77" s="17"/>
+      <c r="G77" s="16"/>
+      <c r="H77" s="16"/>
+    </row>
+    <row r="78" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="11" t="n">
+        <v>34</v>
+      </c>
+      <c r="B78" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="C78" s="6"/>
+      <c r="D78" s="11"/>
+      <c r="E78" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="F78" s="17"/>
+      <c r="G78" s="16"/>
+      <c r="H78" s="16"/>
+    </row>
+    <row r="79" customFormat="false" ht="27.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="11" t="n">
+        <v>35</v>
+      </c>
+      <c r="B79" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="C79" s="6"/>
+      <c r="D79" s="11"/>
+      <c r="E79" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F79" s="17"/>
+      <c r="G79" s="16"/>
+      <c r="H79" s="16"/>
+    </row>
+    <row r="80" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="11" t="n">
+        <v>36</v>
+      </c>
+      <c r="B80" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="C80" s="6"/>
+      <c r="D80" s="11"/>
+      <c r="E80" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F80" s="17"/>
+      <c r="G80" s="16"/>
+      <c r="H80" s="16"/>
+    </row>
+    <row r="81" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="11" t="n">
+        <v>37</v>
+      </c>
+      <c r="B81" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="C81" s="6"/>
+      <c r="D81" s="11"/>
+      <c r="E81" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F81" s="17"/>
+      <c r="G81" s="16"/>
+      <c r="H81" s="16"/>
+    </row>
+    <row r="82" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="11" t="n">
+        <v>38</v>
+      </c>
+      <c r="B82" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C82" s="6"/>
+      <c r="D82" s="11"/>
+      <c r="E82" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="F82" s="17"/>
+      <c r="G82" s="16"/>
+      <c r="H82" s="16"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="C4:C40"/>
+    <mergeCell ref="A44:H44"/>
+    <mergeCell ref="C45:C82"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1712,7 +2508,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1735,7 +2531,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>